<commit_message>
Look OK sur ordi mais pas sur natel. Pas encore de formspree.
</commit_message>
<xml_diff>
--- a/la-cave-de-deuxfoiscinq/carte-des-vins.xlsx
+++ b/la-cave-de-deuxfoiscinq/carte-des-vins.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nico/Sites/deuxfoiscinq/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nico/Sites/deuxfoiscinq/deuxfoiscinq/la-cave-de-deuxfoiscinq/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="14620" windowWidth="51200" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33060" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="CARTE-DES-VINS" sheetId="1" r:id="rId1"/>
+    <sheet name="VIGNERONS" sheetId="2" r:id="rId1"/>
+    <sheet name="CARTE-DES-VINS" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>rivaz</t>
   </si>
@@ -44,9 +45,6 @@
     <t>DOMAINE</t>
   </si>
   <si>
-    <t>VIGNERON</t>
-  </si>
-  <si>
     <t>AOC</t>
   </si>
   <si>
@@ -65,27 +63,12 @@
     <t>saint-saphorin</t>
   </si>
   <si>
-    <t>CÉPAGE</t>
-  </si>
-  <si>
     <t>NOM</t>
   </si>
   <si>
-    <t>INFORMATIONS COMPLÉMENTAIRES</t>
-  </si>
-  <si>
     <t>COULEUR</t>
   </si>
   <si>
-    <t>RÉGION</t>
-  </si>
-  <si>
-    <t>ANNÉE</t>
-  </si>
-  <si>
-    <t>PRIX (CHF/5 dl)</t>
-  </si>
-  <si>
     <t>pinot noir</t>
   </si>
   <si>
@@ -128,7 +111,34 @@
     <t>cornalin</t>
   </si>
   <si>
-    <t>CÉPAGE 2</t>
+    <t>ID_VIGNERON</t>
+  </si>
+  <si>
+    <t>CEPAGE</t>
+  </si>
+  <si>
+    <t>CEPAGE_2</t>
+  </si>
+  <si>
+    <t>REGION</t>
+  </si>
+  <si>
+    <t>ANNEE</t>
+  </si>
+  <si>
+    <t>INFORMATIONS_COMPLEMENTAIRES</t>
+  </si>
+  <si>
+    <t>PRIX</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>http://deuxfoiscinq.ch/blog/bagnoud-vins/</t>
+  </si>
+  <si>
+    <t>http://deuxfoiscinq.ch/blog/rivaz-cave-des-dolles/</t>
   </si>
 </sst>
 </file>
@@ -180,7 +190,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -212,12 +222,55 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="65" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="66">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -233,6 +286,24 @@
     <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -248,11 +319,83 @@
     <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="19">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;CHF&quot;"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -265,21 +408,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:L7" totalsRowShown="0">
-  <autoFilter ref="A1:L7"/>
-  <tableColumns count="12">
-    <tableColumn id="1" name="DOMAINE"/>
-    <tableColumn id="2" name="CAVE"/>
-    <tableColumn id="3" name="VIGNERON"/>
-    <tableColumn id="4" name="AOC"/>
-    <tableColumn id="5" name="CÉPAGE"/>
-    <tableColumn id="6" name="NOM"/>
-    <tableColumn id="7" name="CÉPAGE 2"/>
-    <tableColumn id="8" name="COULEUR"/>
-    <tableColumn id="9" name="RÉGION"/>
-    <tableColumn id="10" name="ANNÉE"/>
-    <tableColumn id="11" name="INFORMATIONS COMPLÉMENTAIRES"/>
-    <tableColumn id="12" name="PRIX (CHF/5 dl)" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:E3" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A1:E3"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="ID_VIGNERON" dataDxfId="6"/>
+    <tableColumn id="4" name="DOMAINE" dataDxfId="5"/>
+    <tableColumn id="2" name="CAVE" dataDxfId="4"/>
+    <tableColumn id="5" name="NOM" dataDxfId="0"/>
+    <tableColumn id="3" name="URL" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:J7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:J7"/>
+  <tableColumns count="10">
+    <tableColumn id="3" name="ID_VIGNERON" dataDxfId="18"/>
+    <tableColumn id="4" name="AOC" dataDxfId="17"/>
+    <tableColumn id="5" name="CEPAGE" dataDxfId="16"/>
+    <tableColumn id="6" name="NOM" dataDxfId="15"/>
+    <tableColumn id="7" name="CEPAGE_2" dataDxfId="14"/>
+    <tableColumn id="8" name="COULEUR" dataDxfId="13"/>
+    <tableColumn id="9" name="REGION" dataDxfId="12"/>
+    <tableColumn id="10" name="ANNEE" dataDxfId="11"/>
+    <tableColumn id="11" name="INFORMATIONS_COMPLEMENTAIRES" dataDxfId="10"/>
+    <tableColumn id="12" name="PRIX" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -548,291 +703,330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2016</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2016</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2016</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="J4" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2015</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
-        <v>18</v>
+      <c r="J5" s="2">
+        <v>10.5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2">
-        <v>2016</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="1">
-        <v>10</v>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2015</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="2">
+        <v>10.5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>2016</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4">
-        <v>2016</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5">
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="1">
         <v>2015</v>
       </c>
-      <c r="K5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="1">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6">
-        <v>2015</v>
-      </c>
-      <c r="K6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="1">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7">
-        <v>2015</v>
-      </c>
-      <c r="K7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="1">
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="2">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ordre des champs fichier Excel formulaire
</commit_message>
<xml_diff>
--- a/la-cave-de-deuxfoiscinq/carte-des-vins.xlsx
+++ b/la-cave-de-deuxfoiscinq/carte-des-vins.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33060" windowHeight="28340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="51120" windowHeight="28360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="VIGNERONS" sheetId="2" r:id="rId1"/>
@@ -364,47 +364,47 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;CHF&quot;"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;CHF&quot;"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
@@ -432,34 +432,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:E3" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau13" displayName="Tableau13" ref="A1:E3" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:E3"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="ID_VIGNERON" dataDxfId="7"/>
-    <tableColumn id="4" name="DOMAINE" dataDxfId="6"/>
-    <tableColumn id="2" name="CAVE" dataDxfId="5"/>
-    <tableColumn id="5" name="NOM" dataDxfId="1"/>
-    <tableColumn id="3" name="URL" dataDxfId="4"/>
+    <tableColumn id="1" name="ID_VIGNERON" dataDxfId="17"/>
+    <tableColumn id="4" name="DOMAINE" dataDxfId="16"/>
+    <tableColumn id="2" name="CAVE" dataDxfId="15"/>
+    <tableColumn id="5" name="NOM" dataDxfId="14"/>
+    <tableColumn id="3" name="URL" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:K7" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:K7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:K7"/>
   <tableColumns count="11">
-    <tableColumn id="3" name="ID_VIGNERON" dataDxfId="19"/>
-    <tableColumn id="4" name="AOC" dataDxfId="18"/>
-    <tableColumn id="5" name="CEPAGE" dataDxfId="17"/>
-    <tableColumn id="6" name="NOM" dataDxfId="16"/>
-    <tableColumn id="7" name="CEPAGE_2" dataDxfId="15"/>
-    <tableColumn id="8" name="COULEUR" dataDxfId="14"/>
-    <tableColumn id="9" name="REGION" dataDxfId="13"/>
-    <tableColumn id="10" name="ANNEE" dataDxfId="12"/>
-    <tableColumn id="11" name="INFORMATIONS_COMPLEMENTAIRES" dataDxfId="11"/>
+    <tableColumn id="3" name="ID_VIGNERON" dataDxfId="10"/>
     <tableColumn id="1" name="REFERENCE" dataDxfId="0"/>
-    <tableColumn id="12" name="PRIX" dataDxfId="10"/>
+    <tableColumn id="4" name="AOC" dataDxfId="9"/>
+    <tableColumn id="5" name="CEPAGE" dataDxfId="8"/>
+    <tableColumn id="6" name="NOM" dataDxfId="7"/>
+    <tableColumn id="7" name="CEPAGE_2" dataDxfId="6"/>
+    <tableColumn id="8" name="COULEUR" dataDxfId="5"/>
+    <tableColumn id="9" name="REGION" dataDxfId="4"/>
+    <tableColumn id="10" name="ANNEE" dataDxfId="3"/>
+    <tableColumn id="11" name="INFORMATIONS_COMPLEMENTAIRES" dataDxfId="2"/>
+    <tableColumn id="12" name="PRIX" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -819,17 +819,18 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="38" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -837,31 +838,31 @@
         <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>33</v>
@@ -872,31 +873,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>2016</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="K2" s="2">
         <v>10</v>
@@ -907,31 +908,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>2016</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="K3" s="2">
         <v>10</v>
@@ -942,31 +943,31 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>2016</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="K4" s="2">
         <v>13</v>
@@ -977,31 +978,31 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>2015</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="K5" s="2">
         <v>10.5</v>
@@ -1012,31 +1013,31 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>2015</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="K6" s="2">
         <v>10.5</v>
@@ -1047,31 +1048,31 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>2015</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="K7" s="2">
         <v>16</v>

</xml_diff>

<commit_message>
modif formulaire de commande (nouvel ID pour les vins remplace ref mail)
</commit_message>
<xml_diff>
--- a/la-cave-de-deuxfoiscinq/carte-des-vins.xlsx
+++ b/la-cave-de-deuxfoiscinq/carte-des-vins.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="112">
   <si>
     <t>rivaz</t>
   </si>
@@ -279,9 +279,6 @@
     <t>http://deuxfoiscinq.ch/blog/praz_bovard/</t>
   </si>
   <si>
-    <t>REFERENCE_MAIL</t>
-  </si>
-  <si>
     <t>COULEUR</t>
   </si>
   <si>
@@ -366,148 +363,7 @@
     <t>×</t>
   </si>
   <si>
-    <t>vin-1</t>
-  </si>
-  <si>
-    <t>vin-2</t>
-  </si>
-  <si>
-    <t>vin-3</t>
-  </si>
-  <si>
-    <t>vin-4</t>
-  </si>
-  <si>
-    <t>vin-5</t>
-  </si>
-  <si>
-    <t>vin-6</t>
-  </si>
-  <si>
-    <t>vin-7</t>
-  </si>
-  <si>
-    <t>vin-8</t>
-  </si>
-  <si>
-    <t>vin-9</t>
-  </si>
-  <si>
-    <t>vin-10</t>
-  </si>
-  <si>
-    <t>vin-11</t>
-  </si>
-  <si>
-    <t>vin-12</t>
-  </si>
-  <si>
-    <t>vin-13</t>
-  </si>
-  <si>
-    <t>vin-14</t>
-  </si>
-  <si>
-    <t>vin-15</t>
-  </si>
-  <si>
-    <t>vin-16</t>
-  </si>
-  <si>
-    <t>vin-17</t>
-  </si>
-  <si>
-    <t>vin-18</t>
-  </si>
-  <si>
-    <t>vin-19</t>
-  </si>
-  <si>
-    <t>vin-20</t>
-  </si>
-  <si>
-    <t>vin-21</t>
-  </si>
-  <si>
-    <t>vin-22</t>
-  </si>
-  <si>
-    <t>vin-23</t>
-  </si>
-  <si>
-    <t>vin-24</t>
-  </si>
-  <si>
-    <t>vin-25</t>
-  </si>
-  <si>
-    <t>vin-26</t>
-  </si>
-  <si>
-    <t>vin-27</t>
-  </si>
-  <si>
-    <t>vin-28</t>
-  </si>
-  <si>
-    <t>vin-29</t>
-  </si>
-  <si>
-    <t>vin-30</t>
-  </si>
-  <si>
-    <t>vin-31</t>
-  </si>
-  <si>
-    <t>vin-32</t>
-  </si>
-  <si>
-    <t>vin-33</t>
-  </si>
-  <si>
-    <t>vin-34</t>
-  </si>
-  <si>
-    <t>vin-35</t>
-  </si>
-  <si>
-    <t>vin-36</t>
-  </si>
-  <si>
-    <t>vin-37</t>
-  </si>
-  <si>
-    <t>vin-38</t>
-  </si>
-  <si>
-    <t>vin-39</t>
-  </si>
-  <si>
-    <t>vin-40</t>
-  </si>
-  <si>
-    <t>vin-41</t>
-  </si>
-  <si>
-    <t>vin-42</t>
-  </si>
-  <si>
-    <t>vin-43</t>
-  </si>
-  <si>
-    <t>vin-44</t>
-  </si>
-  <si>
-    <t>vin-45</t>
-  </si>
-  <si>
-    <t>vin-46</t>
-  </si>
-  <si>
-    <t>vin-47</t>
-  </si>
-  <si>
-    <t>vin-48</t>
+    <t>ID_VIN</t>
   </si>
 </sst>
 </file>
@@ -852,9 +708,6 @@
   </cellStyles>
   <dxfs count="19">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
@@ -898,6 +751,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
@@ -958,15 +814,15 @@
   <autoFilter ref="A1:J50"/>
   <tableColumns count="10">
     <tableColumn id="3" name="ID_VIGNERON" dataDxfId="9"/>
-    <tableColumn id="1" name="REFERENCE_MAIL" dataDxfId="0"/>
-    <tableColumn id="5" name="APPELLATION" dataDxfId="8"/>
-    <tableColumn id="7" name="CEPAGE" dataDxfId="7"/>
-    <tableColumn id="10" name="ANNEE" dataDxfId="6"/>
-    <tableColumn id="8" name="COULEUR" dataDxfId="5"/>
-    <tableColumn id="12" name="PRIX" dataDxfId="4"/>
-    <tableColumn id="6" name="QUANTITE" dataDxfId="3"/>
-    <tableColumn id="2" name="DISPONIBLE" dataDxfId="2"/>
-    <tableColumn id="4" name="REMARQUES" dataDxfId="1"/>
+    <tableColumn id="1" name="ID_VIN" dataDxfId="8"/>
+    <tableColumn id="5" name="APPELLATION" dataDxfId="7"/>
+    <tableColumn id="7" name="CEPAGE" dataDxfId="6"/>
+    <tableColumn id="10" name="ANNEE" dataDxfId="5"/>
+    <tableColumn id="8" name="COULEUR" dataDxfId="4"/>
+    <tableColumn id="12" name="PRIX" dataDxfId="3"/>
+    <tableColumn id="6" name="QUANTITE" dataDxfId="2"/>
+    <tableColumn id="2" name="DISPONIBLE" dataDxfId="1"/>
+    <tableColumn id="4" name="REMARQUES" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1430,13 +1286,13 @@
         <v>52</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1444,16 +1300,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1461,16 +1317,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1504,14 +1360,14 @@
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="169" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="169" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="2" bestFit="1" customWidth="1"/>
@@ -1529,7 +1385,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>72</v>
@@ -1541,7 +1397,7 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>20</v>
@@ -1560,8 +1416,8 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>112</v>
+      <c r="B2" s="2">
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -1573,14 +1429,14 @@
         <v>2016</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2" s="4">
         <v>10</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>56</v>
@@ -1590,8 +1446,8 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>113</v>
+      <c r="B3" s="2">
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -1603,7 +1459,7 @@
         <v>2016</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G3" s="4">
         <v>10</v>
@@ -1616,8 +1472,8 @@
       <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>114</v>
+      <c r="B4" s="2">
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -1629,14 +1485,14 @@
         <v>2016</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G4" s="4">
         <v>13</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>57</v>
@@ -1646,8 +1502,8 @@
       <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>115</v>
+      <c r="B5" s="2">
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>14</v>
@@ -1659,14 +1515,14 @@
         <v>2015</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G5" s="4">
         <v>10.5</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J5" s="4"/>
     </row>
@@ -1674,8 +1530,8 @@
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>116</v>
+      <c r="B6" s="2">
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
@@ -1687,14 +1543,14 @@
         <v>2015</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6" s="4">
         <v>10.5</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J6" s="4"/>
     </row>
@@ -1702,8 +1558,8 @@
       <c r="A7" s="2">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>117</v>
+      <c r="B7" s="2">
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
@@ -1715,14 +1571,14 @@
         <v>2015</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G7" s="4">
         <v>16</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J7" s="4"/>
     </row>
@@ -1730,8 +1586,8 @@
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>118</v>
+      <c r="B8" s="2">
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>24</v>
@@ -1743,14 +1599,14 @@
         <v>2016</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" s="4">
         <v>7.5</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J8" s="4"/>
     </row>
@@ -1758,27 +1614,27 @@
       <c r="A9" s="2">
         <v>3</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>119</v>
+      <c r="B9" s="2">
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" s="2">
         <v>2016</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G9" s="4">
         <v>9.5</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J9" s="4"/>
     </row>
@@ -1786,8 +1642,8 @@
       <c r="A10" s="2">
         <v>3</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>120</v>
+      <c r="B10" s="2">
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
@@ -1799,14 +1655,14 @@
         <v>2016</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G10" s="4">
         <v>10.5</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J10" s="4"/>
     </row>
@@ -1814,8 +1670,8 @@
       <c r="A11" s="1">
         <v>4</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>121</v>
+      <c r="B11" s="2">
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
@@ -1827,7 +1683,7 @@
         <v>2014</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G11" s="4">
         <v>20</v>
@@ -1842,8 +1698,8 @@
       <c r="A12" s="1">
         <v>4</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>122</v>
+      <c r="B12" s="2">
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>27</v>
@@ -1855,7 +1711,7 @@
         <v>2014</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1866,8 +1722,8 @@
       <c r="A13" s="1">
         <v>4</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>123</v>
+      <c r="B13" s="2">
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>27</v>
@@ -1879,14 +1735,14 @@
         <v>2016</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G13" s="4">
         <v>13</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J13" s="4"/>
     </row>
@@ -1894,8 +1750,8 @@
       <c r="A14" s="2">
         <v>5</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>124</v>
+      <c r="B14" s="2">
+        <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>32</v>
@@ -1907,14 +1763,14 @@
         <v>2016</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G14" s="4">
         <v>7.9</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J14" s="4"/>
     </row>
@@ -1922,8 +1778,8 @@
       <c r="A15" s="2">
         <v>5</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>125</v>
+      <c r="B15" s="2">
+        <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>32</v>
@@ -1935,14 +1791,14 @@
         <v>2016</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G15" s="4">
         <v>12</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J15" s="4"/>
     </row>
@@ -1950,8 +1806,8 @@
       <c r="A16" s="2">
         <v>5</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>126</v>
+      <c r="B16" s="2">
+        <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>32</v>
@@ -1963,7 +1819,7 @@
         <v>2016</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G16" s="4">
         <v>12.1</v>
@@ -1976,8 +1832,8 @@
       <c r="A17" s="2">
         <v>5</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>127</v>
+      <c r="B17" s="2">
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>32</v>
@@ -1989,14 +1845,14 @@
         <v>2016</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G17" s="4">
         <v>11.1</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J17" s="4"/>
     </row>
@@ -2004,8 +1860,8 @@
       <c r="A18" s="2">
         <v>6</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>128</v>
+      <c r="B18" s="2">
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>36</v>
@@ -2017,14 +1873,14 @@
         <v>2016</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G18" s="4">
         <v>6.9</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J18" s="4"/>
     </row>
@@ -2032,8 +1888,8 @@
       <c r="A19" s="2">
         <v>6</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>129</v>
+      <c r="B19" s="2">
+        <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>36</v>
@@ -2045,14 +1901,14 @@
         <v>2016</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G19" s="4">
         <v>9.4</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J19" s="4"/>
     </row>
@@ -2060,8 +1916,8 @@
       <c r="A20" s="2">
         <v>6</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>130</v>
+      <c r="B20" s="2">
+        <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>36</v>
@@ -2073,14 +1929,14 @@
         <v>2016</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G20" s="4">
         <v>11.5</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J20" s="4"/>
     </row>
@@ -2088,8 +1944,8 @@
       <c r="A21" s="2">
         <v>7</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>131</v>
+      <c r="B21" s="2">
+        <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>38</v>
@@ -2101,14 +1957,14 @@
         <v>2016</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G21" s="4">
         <v>12.4</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J21" s="4"/>
     </row>
@@ -2116,27 +1972,27 @@
       <c r="A22" s="2">
         <v>7</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>132</v>
+      <c r="B22" s="2">
+        <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E22" s="2">
         <v>2016</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G22" s="4">
         <v>11.3</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J22" s="4"/>
     </row>
@@ -2144,8 +2000,8 @@
       <c r="A23" s="2">
         <v>7</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>133</v>
+      <c r="B23" s="2">
+        <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>38</v>
@@ -2157,14 +2013,14 @@
         <v>2016</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G23" s="4">
         <v>17</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J23" s="4"/>
     </row>
@@ -2172,8 +2028,8 @@
       <c r="A24" s="2">
         <v>8</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>134</v>
+      <c r="B24" s="2">
+        <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>41</v>
@@ -2185,14 +2041,14 @@
         <v>2016</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G24" s="4">
         <v>10.1</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J24" s="4"/>
     </row>
@@ -2200,8 +2056,8 @@
       <c r="A25" s="2">
         <v>8</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>135</v>
+      <c r="B25" s="2">
+        <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>42</v>
@@ -2213,14 +2069,14 @@
         <v>2016</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G25" s="4">
         <v>10.9</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J25" s="4"/>
     </row>
@@ -2228,8 +2084,8 @@
       <c r="A26" s="2">
         <v>8</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>136</v>
+      <c r="B26" s="2">
+        <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>44</v>
@@ -2241,14 +2097,14 @@
         <v>2016</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G26" s="4">
         <v>12.7</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J26" s="4"/>
     </row>
@@ -2256,8 +2112,8 @@
       <c r="A27" s="2">
         <v>8</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>137</v>
+      <c r="B27" s="2">
+        <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>46</v>
@@ -2269,14 +2125,14 @@
         <v>2016</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G27" s="4">
         <v>14</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J27" s="4"/>
     </row>
@@ -2284,8 +2140,8 @@
       <c r="A28" s="2">
         <v>8</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>138</v>
+      <c r="B28" s="2">
+        <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>42</v>
@@ -2297,7 +2153,7 @@
         <v>2016</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G28" s="4">
         <v>11.6</v>
@@ -2310,8 +2166,8 @@
       <c r="A29" s="2">
         <v>9</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>139</v>
+      <c r="B29" s="2">
+        <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>50</v>
@@ -2323,14 +2179,14 @@
         <v>2016</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G29" s="4">
         <v>8.5</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J29" s="4"/>
     </row>
@@ -2338,27 +2194,27 @@
       <c r="A30" s="2">
         <v>9</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>140</v>
+      <c r="B30" s="2">
+        <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E30" s="2">
         <v>2016</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G30" s="4">
         <v>11.5</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J30" s="4"/>
     </row>
@@ -2366,8 +2222,8 @@
       <c r="A31" s="2">
         <v>9</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>141</v>
+      <c r="B31" s="2">
+        <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>50</v>
@@ -2379,14 +2235,14 @@
         <v>2016</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G31" s="4">
         <v>12.5</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J31" s="4"/>
     </row>
@@ -2394,8 +2250,8 @@
       <c r="A32" s="2">
         <v>9</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>142</v>
+      <c r="B32" s="2">
+        <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>50</v>
@@ -2407,7 +2263,7 @@
         <v>2016</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G32" s="4">
         <v>12.5</v>
@@ -2420,8 +2276,8 @@
       <c r="A33" s="2">
         <v>10</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>143</v>
+      <c r="B33" s="2">
+        <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>52</v>
@@ -2433,7 +2289,7 @@
         <v>2016</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G33" s="4">
         <v>6.5</v>
@@ -2446,8 +2302,8 @@
       <c r="A34" s="2">
         <v>10</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>144</v>
+      <c r="B34" s="2">
+        <v>33</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>52</v>
@@ -2459,7 +2315,7 @@
         <v>2016</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G34" s="4">
         <v>7</v>
@@ -2472,8 +2328,8 @@
       <c r="A35" s="2">
         <v>10</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>145</v>
+      <c r="B35" s="2">
+        <v>34</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>52</v>
@@ -2485,7 +2341,7 @@
         <v>2016</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G35" s="4">
         <v>8</v>
@@ -2498,20 +2354,20 @@
       <c r="A36" s="2">
         <v>10</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>146</v>
+      <c r="B36" s="2">
+        <v>35</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E36" s="2">
         <v>2016</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G36" s="4">
         <v>8</v>
@@ -2524,8 +2380,8 @@
       <c r="A37" s="2">
         <v>10</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>147</v>
+      <c r="B37" s="2">
+        <v>36</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>52</v>
@@ -2537,7 +2393,7 @@
         <v>2016</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G37" s="4">
         <v>8.5</v>
@@ -2550,27 +2406,27 @@
       <c r="A38" s="2">
         <v>11</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>148</v>
+      <c r="B38" s="2">
+        <v>37</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E38" s="2">
         <v>2016</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G38" s="4">
         <v>11</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J38" s="2"/>
     </row>
@@ -2578,27 +2434,27 @@
       <c r="A39" s="2">
         <v>11</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>148</v>
+      <c r="B39" s="2">
+        <v>38</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E39" s="2">
         <v>2016</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G39" s="4">
         <v>11.7</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J39" s="2"/>
     </row>
@@ -2606,27 +2462,27 @@
       <c r="A40" s="2">
         <v>11</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>149</v>
+      <c r="B40" s="2">
+        <v>39</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" s="2">
+        <v>2016</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="E40" s="2">
-        <v>2016</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="G40" s="4">
         <v>12.8</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J40" s="2"/>
     </row>
@@ -2634,27 +2490,27 @@
       <c r="A41" s="2">
         <v>11</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>150</v>
+      <c r="B41" s="2">
+        <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E41" s="2">
         <v>2016</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G41" s="4">
         <v>18</v>
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J41" s="2"/>
     </row>
@@ -2662,27 +2518,27 @@
       <c r="A42" s="2">
         <v>12</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>151</v>
+      <c r="B42" s="2">
+        <v>41</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E42" s="2">
         <v>2016</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G42" s="4">
         <v>6.5</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J42" s="2"/>
     </row>
@@ -2690,27 +2546,27 @@
       <c r="A43" s="2">
         <v>12</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>152</v>
+      <c r="B43" s="2">
+        <v>42</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E43" s="2">
         <v>2016</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G43" s="4">
         <v>9.5</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J43" s="2"/>
     </row>
@@ -2718,20 +2574,20 @@
       <c r="A44" s="2">
         <v>12</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>153</v>
+      <c r="B44" s="2">
+        <v>43</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E44" s="2">
         <v>2016</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G44" s="4">
         <v>12.5</v>
@@ -2744,27 +2600,27 @@
       <c r="A45" s="2">
         <v>12</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>154</v>
+      <c r="B45" s="2">
+        <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E45" s="2">
         <v>2016</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G45" s="4">
         <v>7.5</v>
       </c>
       <c r="H45" s="4"/>
       <c r="I45" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J45" s="2"/>
     </row>
@@ -2772,11 +2628,11 @@
       <c r="A46" s="2">
         <v>12</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>155</v>
+      <c r="B46" s="2">
+        <v>45</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>8</v>
@@ -2785,14 +2641,14 @@
         <v>2015</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G46" s="4">
         <v>9.5</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J46" s="2"/>
     </row>
@@ -2800,27 +2656,27 @@
       <c r="A47" s="2">
         <v>12</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>156</v>
+      <c r="B47" s="2">
+        <v>46</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E47" s="2">
         <v>2016</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G47" s="4">
         <v>10</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J47" s="2"/>
     </row>
@@ -2828,27 +2684,27 @@
       <c r="A48" s="2">
         <v>12</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>157</v>
+      <c r="B48" s="2">
+        <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E48" s="2">
         <v>2015</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G48" s="4">
         <v>13.5</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J48" s="2"/>
     </row>
@@ -2856,11 +2712,11 @@
       <c r="A49" s="2">
         <v>12</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>158</v>
+      <c r="B49" s="2">
+        <v>48</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>51</v>
@@ -2869,14 +2725,14 @@
         <v>2015</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G49" s="4">
         <v>13.5</v>
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J49" s="2"/>
     </row>
@@ -2884,27 +2740,27 @@
       <c r="A50" s="2">
         <v>12</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>159</v>
+      <c r="B50" s="2">
+        <v>49</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E50" s="2">
         <v>2016</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G50" s="4">
         <v>8.5</v>
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J50" s="2"/>
     </row>

</xml_diff>

<commit_message>
mis tous les vins de soral en “disponible”
</commit_message>
<xml_diff>
--- a/la-cave-de-deuxfoiscinq/carte-des-vins.xlsx
+++ b/la-cave-de-deuxfoiscinq/carte-des-vins.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nico/Sites/deuxfoiscinq/deuxfoiscinq/la-cave-de-deuxfoiscinq/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="51120" windowHeight="28360" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="VIGNERONS" sheetId="2" r:id="rId1"/>
@@ -12,18 +17,18 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="111">
   <si>
     <t>rivaz</t>
   </si>
@@ -1075,7 +1080,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1086,11 +1091,11 @@
   <sheetPr codeName="Feuille1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="169" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="169" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" style="7" customWidth="1"/>
@@ -1100,7 +1105,7 @@
     <col min="6" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -1117,7 +1122,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1134,7 +1139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1151,7 +1156,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1168,7 +1173,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1185,7 +1190,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1202,7 +1207,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1219,7 +1224,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1236,7 +1241,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1253,7 +1258,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1270,7 +1275,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>-10</v>
       </c>
@@ -1287,7 +1292,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1304,7 +1309,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1342,11 +1347,6 @@
   <tableParts count="1">
     <tablePart r:id="rId13"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1357,11 +1357,11 @@
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="169" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="169" zoomScaleNormal="169" zoomScalePageLayoutView="169" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="2" bestFit="1" customWidth="1"/>
@@ -1377,7 +1377,7 @@
     <col min="12" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1465,7 +1465,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1523,7 +1523,7 @@
       </c>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>3</v>
       </c>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>3</v>
       </c>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -1715,7 +1715,7 @@
       <c r="I12" s="10"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -1743,7 +1743,7 @@
       </c>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="J14" s="4"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>5</v>
       </c>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>5</v>
       </c>
@@ -1825,7 +1825,7 @@
       <c r="I16" s="10"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>5</v>
       </c>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>6</v>
       </c>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>6</v>
       </c>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>6</v>
       </c>
@@ -1937,7 +1937,7 @@
       </c>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>7</v>
       </c>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="J21" s="4"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>7</v>
       </c>
@@ -1993,7 +1993,7 @@
       </c>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>7</v>
       </c>
@@ -2021,7 +2021,7 @@
       </c>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>8</v>
       </c>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>8</v>
       </c>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>8</v>
       </c>
@@ -2105,7 +2105,7 @@
       </c>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>8</v>
       </c>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>8</v>
       </c>
@@ -2159,7 +2159,7 @@
       <c r="I28" s="10"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>9</v>
       </c>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>9</v>
       </c>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>9</v>
       </c>
@@ -2243,7 +2243,7 @@
       </c>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>9</v>
       </c>
@@ -2269,7 +2269,7 @@
       <c r="I32" s="10"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>10</v>
       </c>
@@ -2295,7 +2295,7 @@
       <c r="I33" s="11"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>10</v>
       </c>
@@ -2321,7 +2321,7 @@
       <c r="I34" s="10"/>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>10</v>
       </c>
@@ -2347,7 +2347,7 @@
       <c r="I35" s="11"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>10</v>
       </c>
@@ -2373,7 +2373,7 @@
       <c r="I36" s="10"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>10</v>
       </c>
@@ -2399,7 +2399,7 @@
       <c r="I37" s="11"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>11</v>
       </c>
@@ -2427,7 +2427,7 @@
       </c>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>11</v>
       </c>
@@ -2455,7 +2455,7 @@
       </c>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>11</v>
       </c>
@@ -2481,7 +2481,7 @@
       <c r="I40" s="11"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>11</v>
       </c>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>12</v>
       </c>
@@ -2532,10 +2532,12 @@
         <v>6.5</v>
       </c>
       <c r="H42" s="4"/>
-      <c r="I42" s="11"/>
+      <c r="I42" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>12</v>
       </c>
@@ -2558,10 +2560,12 @@
         <v>9.5</v>
       </c>
       <c r="H43" s="4"/>
-      <c r="I43" s="11"/>
+      <c r="I43" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>12</v>
       </c>
@@ -2584,10 +2588,12 @@
         <v>12.5</v>
       </c>
       <c r="H44" s="4"/>
-      <c r="I44" s="10"/>
+      <c r="I44" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>12</v>
       </c>
@@ -2610,10 +2616,12 @@
         <v>7.5</v>
       </c>
       <c r="H45" s="4"/>
-      <c r="I45" s="11"/>
+      <c r="I45" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>12</v>
       </c>
@@ -2636,10 +2644,12 @@
         <v>9.5</v>
       </c>
       <c r="H46" s="4"/>
-      <c r="I46" s="11"/>
+      <c r="I46" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>12</v>
       </c>
@@ -2662,10 +2672,12 @@
         <v>10</v>
       </c>
       <c r="H47" s="4"/>
-      <c r="I47" s="11"/>
+      <c r="I47" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>12</v>
       </c>
@@ -2688,10 +2700,12 @@
         <v>13.5</v>
       </c>
       <c r="H48" s="4"/>
-      <c r="I48" s="11"/>
+      <c r="I48" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>12</v>
       </c>
@@ -2714,10 +2728,12 @@
         <v>13.5</v>
       </c>
       <c r="H49" s="4"/>
-      <c r="I49" s="11"/>
+      <c r="I49" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>12</v>
       </c>
@@ -2740,7 +2756,9 @@
         <v>8.5</v>
       </c>
       <c r="H50" s="4"/>
-      <c r="I50" s="11"/>
+      <c r="I50" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="J50" s="2"/>
     </row>
   </sheetData>
@@ -2750,10 +2768,5 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>